<commit_message>
Updates to Botswana workflows for lab order patient matching. (#104)
* Version Bump

* Pilot work

* Updates for bdrs/immigration matching for Botswana

* HL7 retry DMQ and sender updates

* Build fixes

* Dep update
</commit_message>
<xml_diff>
--- a/config/ipms_facility_mappings.xlsx
+++ b/config/ipms_facility_mappings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3e0149e38b7073bf/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piotr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{35E1EDCB-15B4-4482-A91E-109A57F47F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6ACF6D35-CD5D-4C49-8054-BD2A5B69FB1E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AE3AF1-ED14-4BF7-A9BC-583765CCDAC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,14 +391,14 @@
     <t>BLL</t>
   </si>
   <si>
-    <t>Airstrip Clinic</t>
+    <t>Air Strip Clinic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -443,6 +443,12 @@
       <sz val="10"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -541,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -592,6 +598,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -814,7 +821,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
+      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2273,7 +2280,7 @@
       <c r="D42" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="E42" s="21" t="s">
+      <c r="E42" s="26" t="s">
         <v>60</v>
       </c>
       <c r="F42" s="6" t="s">
@@ -3990,6 +3997,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>